<commit_message>
Avoid duplicate Amoxicillin medicines.
</commit_message>
<xml_diff>
--- a/scripts/country_visit/data/zambia_framework_contract_cleaned.xlsx
+++ b/scripts/country_visit/data/zambia_framework_contract_cleaned.xlsx
@@ -170,9 +170,6 @@
     <t>Amoxicillin + capsule + 250 mg</t>
   </si>
   <si>
-    <t>Amoxycillin + powder for suspension + 125 mg/5ml + 100ml</t>
-  </si>
-  <si>
     <t>Ampicillin + powder for injection + 500 mg</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>Vincristine Sulphate + Injection + 1 mg/ml + + liquid</t>
+  </si>
+  <si>
+    <t>Amoxicillin + powder for suspension + 125 mg/5ml + 100ml</t>
   </si>
 </sst>
 </file>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1208,7 +1208,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="C9" s="15">
         <v>1</v>
@@ -1234,7 +1234,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
@@ -1260,7 +1260,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="15">
         <v>1</v>
@@ -1286,7 +1286,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="15">
         <v>1</v>
@@ -1310,7 +1310,7 @@
     <row r="13" spans="1:8" ht="20" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="15">
         <v>1000</v>
@@ -1336,7 +1336,7 @@
         <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="15">
         <v>1</v>
@@ -1362,7 +1362,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
@@ -1388,7 +1388,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="15">
         <v>1</v>
@@ -1414,7 +1414,7 @@
         <v>123</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
@@ -1440,7 +1440,7 @@
         <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
@@ -1455,7 +1455,7 @@
         <v>18</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H18" s="13">
         <v>1</v>
@@ -1466,7 +1466,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="15">
         <v>1000</v>
@@ -1518,7 +1518,7 @@
         <v>124</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="15">
         <v>1</v>
@@ -1544,7 +1544,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="15">
         <v>1000</v>
@@ -1570,7 +1570,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="15">
         <v>1</v>
@@ -1596,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="15">
         <v>1</v>
@@ -1611,7 +1611,7 @@
         <v>20</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H24" s="13">
         <v>1</v>
@@ -1620,7 +1620,7 @@
     <row r="25" spans="1:8" ht="20" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="15">
         <v>1000</v>
@@ -1646,7 +1646,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="15">
         <v>1</v>
@@ -1672,7 +1672,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="15">
         <v>1000</v>
@@ -1696,7 +1696,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="15">
         <v>1</v>
@@ -1720,7 +1720,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="15">
         <v>1000</v>
@@ -1746,7 +1746,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="15">
         <v>1</v>
@@ -1770,7 +1770,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="15">
         <v>1000</v>
@@ -1794,7 +1794,7 @@
         <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="15">
         <v>1</v>
@@ -1820,7 +1820,7 @@
         <v>116</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" s="15">
         <v>1</v>
@@ -1844,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="15">
         <v>1</v>
@@ -1870,7 +1870,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="15">
         <v>1000</v>
@@ -1896,7 +1896,7 @@
         <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="15">
         <v>1</v>
@@ -1922,7 +1922,7 @@
         <v>56</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="15">
         <v>100</v>
@@ -1948,7 +1948,7 @@
         <v>51</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="15">
         <v>1000</v>
@@ -1972,7 +1972,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="15">
         <v>1</v>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="13">
         <v>1</v>
@@ -1996,7 +1996,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="15">
         <v>1000</v>
@@ -2022,7 +2022,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="15">
         <v>1</v>
@@ -2048,7 +2048,7 @@
         <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="15">
         <v>1</v>
@@ -2072,7 +2072,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" s="15">
         <v>100</v>
@@ -2098,7 +2098,7 @@
         <v>45</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="15">
         <v>1</v>
@@ -2124,7 +2124,7 @@
         <v>64</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="15">
         <v>1</v>
@@ -2150,7 +2150,7 @@
         <v>62</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="15">
         <v>1000</v>
@@ -2176,7 +2176,7 @@
         <v>37</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="16">
         <v>1</v>
@@ -2202,7 +2202,7 @@
         <v>72</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" s="15">
         <v>1</v>
@@ -2226,7 +2226,7 @@
         <v>82</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="15">
         <v>1</v>
@@ -2252,7 +2252,7 @@
         <v>46</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" s="15">
         <v>1</v>
@@ -2278,7 +2278,7 @@
         <v>60</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51" s="15">
         <v>1</v>
@@ -2304,7 +2304,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="15">
         <v>1000</v>
@@ -2330,7 +2330,7 @@
         <v>74</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="15">
         <v>1</v>
@@ -2345,7 +2345,7 @@
         <v>30</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H53" s="13">
         <v>15</v>
@@ -2356,7 +2356,7 @@
         <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C54" s="15">
         <v>1</v>
@@ -2380,7 +2380,7 @@
         <v>11</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="15">
         <v>1</v>
@@ -2406,7 +2406,7 @@
         <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C56" s="15">
         <v>1</v>
@@ -2430,7 +2430,7 @@
         <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" s="15">
         <v>100</v>
@@ -2452,7 +2452,7 @@
     <row r="58" spans="1:8" ht="20" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C58" s="15">
         <v>1000</v>
@@ -2478,7 +2478,7 @@
         <v>152</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" s="15">
         <v>1</v>
@@ -2502,7 +2502,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" s="15">
         <v>1</v>
@@ -2528,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C61" s="15">
         <v>1</v>
@@ -2554,7 +2554,7 @@
         <v>98</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C62" s="15">
         <v>1000</v>
@@ -2578,7 +2578,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" s="15">
         <v>1000</v>
@@ -2604,7 +2604,7 @@
         <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C64" s="15">
         <v>1</v>
@@ -2630,7 +2630,7 @@
         <v>102</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C65" s="15">
         <v>1000</v>
@@ -2654,7 +2654,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C66" s="15">
         <v>1</v>
@@ -2680,7 +2680,7 @@
         <v>103</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67" s="16">
         <v>1000</v>
@@ -2704,7 +2704,7 @@
         <v>55</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" s="15">
         <v>1000</v>
@@ -2728,7 +2728,7 @@
         <v>95</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C69" s="15">
         <v>1</v>
@@ -2754,7 +2754,7 @@
         <v>104</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C70" s="16">
         <v>1</v>
@@ -2778,7 +2778,7 @@
         <v>17</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C71" s="15">
         <v>1000</v>
@@ -2804,7 +2804,7 @@
         <v>106</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C72" s="15">
         <v>1</v>
@@ -2830,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C73" s="15">
         <v>500</v>
@@ -2854,7 +2854,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C74" s="15">
         <v>1</v>
@@ -2880,7 +2880,7 @@
         <v>12</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C75" s="15">
         <v>1</v>
@@ -2904,7 +2904,7 @@
         <v>70</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C76" s="15">
         <v>1</v>
@@ -2930,7 +2930,7 @@
         <v>96</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C77" s="15">
         <v>1</v>
@@ -2954,7 +2954,7 @@
         <v>109</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C78" s="15">
         <v>1000</v>
@@ -2980,7 +2980,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C79" s="15">
         <v>1000</v>
@@ -3004,7 +3004,7 @@
         <v>67</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C80" s="15">
         <v>1000</v>
@@ -3030,7 +3030,7 @@
         <v>92</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C81" s="15">
         <v>1000</v>
@@ -3056,7 +3056,7 @@
         <v>48</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C82" s="15">
         <v>1</v>
@@ -3080,7 +3080,7 @@
         <v>65</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C83" s="15">
         <v>1</v>
@@ -3104,7 +3104,7 @@
         <v>78</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C84" s="16">
         <v>1</v>
@@ -3128,7 +3128,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C85" s="16">
         <v>100</v>
@@ -3152,7 +3152,7 @@
         <v>108</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C86" s="15">
         <v>1</v>
@@ -3178,7 +3178,7 @@
         <v>107</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C87" s="15">
         <v>1</v>
@@ -3204,7 +3204,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C88" s="15">
         <v>1000</v>
@@ -3230,7 +3230,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C89" s="15">
         <v>1000</v>
@@ -3256,7 +3256,7 @@
         <v>4</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C90" s="15">
         <v>1000</v>
@@ -3282,7 +3282,7 @@
         <v>5</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C91" s="15">
         <v>1</v>
@@ -3297,7 +3297,7 @@
         <v>22</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H91" s="13">
         <v>5</v>
@@ -3308,7 +3308,7 @@
         <v>6</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C92" s="15">
         <v>1</v>
@@ -3334,7 +3334,7 @@
         <v>7</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C93" s="15">
         <v>1000</v>
@@ -3360,7 +3360,7 @@
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C94" s="15">
         <v>1</v>
@@ -3386,7 +3386,7 @@
         <v>9</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C95" s="15">
         <v>1</v>
@@ -3412,7 +3412,7 @@
         <v>10</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C96" s="15">
         <v>10</v>
@@ -3438,7 +3438,7 @@
         <v>11</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C97" s="15">
         <v>1</v>
@@ -3464,7 +3464,7 @@
         <v>12</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C98" s="15">
         <v>1000</v>
@@ -3490,7 +3490,7 @@
         <v>13</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C99" s="15">
         <v>1</v>
@@ -3516,7 +3516,7 @@
         <v>14</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C100" s="15">
         <v>1</v>
@@ -3542,7 +3542,7 @@
         <v>15</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C101" s="15">
         <v>1</v>

</xml_diff>